<commit_message>
pages updated and create community testcase
</commit_message>
<xml_diff>
--- a/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
@@ -38,25 +38,25 @@
     <t xml:space="preserve">Warke</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel Info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEX Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 3</t>
+    <t xml:space="preserve">Channel Name .0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel Type .1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel Info .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEX Color .3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 1   .4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 2   .5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 3  .6</t>
   </si>
   <si>
     <t xml:space="preserve">Channel owner name</t>
@@ -328,21 +328,23 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="13.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="5" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="21.26"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="5" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
update write excel data file
</commit_message>
<xml_diff>
--- a/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Channel" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Discover" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
@@ -75,6 +76,18 @@
   </si>
   <si>
     <t xml:space="preserve">#11ee62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Followers</t>
   </si>
 </sst>
 </file>
@@ -156,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -183,6 +196,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -327,7 +344,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -337,9 +354,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="21.26"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="5" width="11.52"/>
   </cols>
@@ -385,6 +402,50 @@
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in follw chnl tc edit channel profile drawer page added excel sheet updated edit channel tc created-incomplete
</commit_message>
<xml_diff>
--- a/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
@@ -39,25 +39,28 @@
     <t xml:space="preserve">Warke</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel Name .0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel Type .1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel Info .2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEX Color .3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 1   .4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 2   .5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 3  .6</t>
+    <t xml:space="preserve">col no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel Name .1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel Type .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel Info .3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEX Color .4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 1   .5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 2   .6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 3  .7</t>
   </si>
   <si>
     <t xml:space="preserve">Channel owner name</t>
@@ -66,6 +69,9 @@
     <t xml:space="preserve">Channel owner mob</t>
   </si>
   <si>
+    <t xml:space="preserve">NOTE</t>
+  </si>
+  <si>
     <t xml:space="preserve">KrushiPradhan Desh</t>
   </si>
   <si>
@@ -76,6 +82,15 @@
   </si>
   <si>
     <t xml:space="preserve">#11ee62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For create channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ee1111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For edit channel profile</t>
   </si>
   <si>
     <t xml:space="preserve">Count</t>
@@ -98,7 +113,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -120,8 +135,15 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,8 +156,20 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEDCC6"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -143,6 +177,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -169,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,12 +238,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -215,7 +279,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -252,7 +316,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFEDCC6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -282,7 +346,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -342,66 +406,198 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="21.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="16.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="6" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="K1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -422,7 +618,7 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -435,17 +631,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>21</v>
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit channel profile TC done
</commit_message>
<xml_diff>
--- a/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
+++ b/KISANCHAT/src/test/java/TestData/ExcelData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t xml:space="preserve">Mobile Number</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">For create channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KrushiPradhan DeshEdited</t>
   </si>
   <si>
     <t xml:space="preserve">#ee1111</t>
@@ -409,7 +412,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,12 +488,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>17</v>
@@ -499,10 +502,10 @@
         <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,16 +635,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>